<commit_message>
Security implemented but not yet tested.
</commit_message>
<xml_diff>
--- a/Urenstaat-2018.xlsx
+++ b/Urenstaat-2018.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>Dit werkblad hebben wij aangemaakt om te kunnen controleren of de gratis producten van Easy Template niet onrechtmatig worden gekopieerd</t>
   </si>
@@ -154,6 +154,33 @@
   </si>
   <si>
     <t>verdieping in estimote API</t>
+  </si>
+  <si>
+    <t>Build process impl</t>
+  </si>
+  <si>
+    <t>Jenkins install</t>
+  </si>
+  <si>
+    <t>Nexus install</t>
+  </si>
+  <si>
+    <t>build process implementation</t>
+  </si>
+  <si>
+    <t>Pipeline defination</t>
+  </si>
+  <si>
+    <t>Database definition</t>
+  </si>
+  <si>
+    <t>Security implementation</t>
+  </si>
+  <si>
+    <t>MySql error</t>
+  </si>
+  <si>
+    <t>Entity defination</t>
   </si>
 </sst>
 </file>
@@ -356,13 +383,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
@@ -414,6 +452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -435,10 +474,20 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1"/>
@@ -986,13 +1035,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="C142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomRight" activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1008,11 +1057,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:7">
       <c r="D7" s="7"/>
@@ -1025,9 +1074,9 @@
         <v>12</v>
       </c>
       <c r="F8" s="24"/>
-      <c r="G8" s="33">
-        <f>SUM(F16:F72)</f>
-        <v>42</v>
+      <c r="G8" s="25">
+        <f>SUM(F16:F300)</f>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1107,7 +1156,7 @@
         <v>43103</v>
       </c>
       <c r="B15" s="15" t="str">
-        <f t="shared" ref="B15:B72" si="1">IF(A15="","",TEXT(A15,"dddd"))</f>
+        <f t="shared" ref="B15:B78" si="1">IF(A15="","",TEXT(A15,"dddd"))</f>
         <v>Wednesday</v>
       </c>
       <c r="C15" s="4"/>
@@ -1683,7 +1732,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E47" s="14">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="F47" s="15">
         <v>4</v>
@@ -1889,12 +1938,18 @@
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="E60" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F60" s="15">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1905,12 +1960,18 @@
         <f t="shared" si="1"/>
         <v>Sunday</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C61" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E61" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F61" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2001,12 +2062,18 @@
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C67" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="E67" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F67" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2017,12 +2084,18 @@
         <f t="shared" si="1"/>
         <v>Sunday</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C68" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="E68" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F68" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2086,6 +2159,1918 @@
       <c r="E72" s="14"/>
       <c r="F72" s="15" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="13">
+        <v>43161</v>
+      </c>
+      <c r="B73" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Friday</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="15" t="str">
+        <f t="shared" ref="F73:F101" si="2">IF(E73="","",IF(D73="","",IF(E73&lt;D73,ROUND((E73-D73)*24,2)+24,ROUND((E73-D73)*24,2))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="13">
+        <v>43162</v>
+      </c>
+      <c r="B74" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="E74" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F74" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="13">
+        <v>43163</v>
+      </c>
+      <c r="B75" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E75" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F75" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="13">
+        <v>43164</v>
+      </c>
+      <c r="B76" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Monday</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D76" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E76" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F76" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="13">
+        <v>43165</v>
+      </c>
+      <c r="B77" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E77" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F77" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="13">
+        <v>43166</v>
+      </c>
+      <c r="B78" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E78" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F78" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="13">
+        <v>43167</v>
+      </c>
+      <c r="B79" s="15" t="str">
+        <f t="shared" ref="B79:B142" si="3">IF(A79="","",TEXT(A79,"dddd"))</f>
+        <v>Thursday</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E79" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F79" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="13">
+        <v>43168</v>
+      </c>
+      <c r="B80" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E80" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F80" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="13">
+        <v>43169</v>
+      </c>
+      <c r="B81" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E81" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F81" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="13">
+        <v>43170</v>
+      </c>
+      <c r="B82" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="15" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="13">
+        <v>43171</v>
+      </c>
+      <c r="B83" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E83" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F83" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="13">
+        <v>43172</v>
+      </c>
+      <c r="B84" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E84" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F84" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="13">
+        <v>43173</v>
+      </c>
+      <c r="B85" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D85" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E85" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F85" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="13">
+        <v>43174</v>
+      </c>
+      <c r="B86" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D86" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E86" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F86" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="13">
+        <v>43175</v>
+      </c>
+      <c r="B87" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D87" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E87" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F87" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="13">
+        <v>43176</v>
+      </c>
+      <c r="B88" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D88" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E88" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F88" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="13">
+        <v>43177</v>
+      </c>
+      <c r="B89" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D89" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E89" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F89" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="13">
+        <v>43178</v>
+      </c>
+      <c r="B90" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D90" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E90" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F90" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="13">
+        <v>43179</v>
+      </c>
+      <c r="B91" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D91" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E91" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F91" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="13">
+        <v>43180</v>
+      </c>
+      <c r="B92" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D92" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E92" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F92" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="13">
+        <v>43181</v>
+      </c>
+      <c r="B93" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D93" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E93" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F93" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="13">
+        <v>43182</v>
+      </c>
+      <c r="B94" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D94" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E94" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F94" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="13">
+        <v>43183</v>
+      </c>
+      <c r="B95" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D95" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E95" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F95" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="13">
+        <v>43184</v>
+      </c>
+      <c r="B96" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D96" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E96" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F96" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="13">
+        <v>43185</v>
+      </c>
+      <c r="B97" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D97" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E97" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F97" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="13">
+        <v>43186</v>
+      </c>
+      <c r="B98" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D98" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E98" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F98" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="13">
+        <v>43187</v>
+      </c>
+      <c r="B99" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D99" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E99" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F99" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="13">
+        <v>43188</v>
+      </c>
+      <c r="B100" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D100" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E100" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F100" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="13">
+        <v>43189</v>
+      </c>
+      <c r="B101" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D101" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E101" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F101" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="13">
+        <v>43190</v>
+      </c>
+      <c r="B102" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D102" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E102" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F102" s="15">
+        <f t="shared" ref="F102:F160" si="4">IF(E102="","",IF(D102="","",IF(E102&lt;D102,ROUND((E102-D102)*24,2)+24,ROUND((E102-D102)*24,2))))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="13">
+        <v>43191</v>
+      </c>
+      <c r="B103" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D103" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E103" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F103" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="13">
+        <v>43192</v>
+      </c>
+      <c r="B104" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E104" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F104" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="13">
+        <v>43193</v>
+      </c>
+      <c r="B105" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D105" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E105" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F105" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="13">
+        <v>43194</v>
+      </c>
+      <c r="B106" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D106" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E106" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F106" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="13">
+        <v>43195</v>
+      </c>
+      <c r="B107" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D107" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E107" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F107" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="13">
+        <v>43196</v>
+      </c>
+      <c r="B108" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D108" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E108" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F108" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="13">
+        <v>43197</v>
+      </c>
+      <c r="B109" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D109" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E109" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F109" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="13">
+        <v>43198</v>
+      </c>
+      <c r="B110" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D110" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E110" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F110" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="13">
+        <v>43199</v>
+      </c>
+      <c r="B111" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D111" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E111" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F111" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="13">
+        <v>43200</v>
+      </c>
+      <c r="B112" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D112" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E112" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F112" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="13">
+        <v>43201</v>
+      </c>
+      <c r="B113" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D113" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E113" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F113" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="13">
+        <v>43202</v>
+      </c>
+      <c r="B114" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D114" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E114" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F114" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="13">
+        <v>43203</v>
+      </c>
+      <c r="B115" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D115" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E115" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F115" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="13">
+        <v>43204</v>
+      </c>
+      <c r="B116" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D116" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E116" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F116" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="13">
+        <v>43205</v>
+      </c>
+      <c r="B117" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D117" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E117" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F117" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="13">
+        <v>43206</v>
+      </c>
+      <c r="B118" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D118" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E118" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F118" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="13">
+        <v>43207</v>
+      </c>
+      <c r="B119" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D119" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E119" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F119" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="13">
+        <v>43208</v>
+      </c>
+      <c r="B120" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D120" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E120" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F120" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="13">
+        <v>43209</v>
+      </c>
+      <c r="B121" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D121" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E121" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F121" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="13">
+        <v>43210</v>
+      </c>
+      <c r="B122" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D122" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E122" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F122" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="13">
+        <v>43211</v>
+      </c>
+      <c r="B123" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E123" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F123" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="13">
+        <v>43212</v>
+      </c>
+      <c r="B124" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D124" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E124" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F124" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="13">
+        <v>43213</v>
+      </c>
+      <c r="B125" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D125" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E125" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F125" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="13">
+        <v>43214</v>
+      </c>
+      <c r="B126" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D126" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E126" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F126" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="13">
+        <v>43215</v>
+      </c>
+      <c r="B127" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D127" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E127" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F127" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="13">
+        <v>43216</v>
+      </c>
+      <c r="B128" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D128" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E128" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F128" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="13">
+        <v>43217</v>
+      </c>
+      <c r="B129" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D129" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E129" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F129" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="13">
+        <v>43218</v>
+      </c>
+      <c r="B130" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D130" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E130" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F130" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="13">
+        <v>43219</v>
+      </c>
+      <c r="B131" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D131" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E131" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F131" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="13">
+        <v>43220</v>
+      </c>
+      <c r="B132" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D132" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E132" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F132" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="13">
+        <v>43221</v>
+      </c>
+      <c r="B133" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D133" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E133" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F133" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="13">
+        <v>43222</v>
+      </c>
+      <c r="B134" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D134" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E134" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F134" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="13">
+        <v>43223</v>
+      </c>
+      <c r="B135" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D135" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E135" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F135" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="13">
+        <v>43224</v>
+      </c>
+      <c r="B136" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D136" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E136" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F136" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="13">
+        <v>43225</v>
+      </c>
+      <c r="B137" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D137" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E137" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F137" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="13">
+        <v>43226</v>
+      </c>
+      <c r="B138" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D138" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E138" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F138" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="13">
+        <v>43227</v>
+      </c>
+      <c r="B139" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Monday</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D139" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E139" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F139" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="13">
+        <v>43228</v>
+      </c>
+      <c r="B140" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D140" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E140" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F140" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="13">
+        <v>43229</v>
+      </c>
+      <c r="B141" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D141" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E141" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F141" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="13">
+        <v>43230</v>
+      </c>
+      <c r="B142" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D142" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E142" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F142" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="13">
+        <v>43231</v>
+      </c>
+      <c r="B143" s="15" t="str">
+        <f t="shared" ref="B143:B161" si="5">IF(A143="","",TEXT(A143,"dddd"))</f>
+        <v>Friday</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E143" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F143" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="13">
+        <v>43232</v>
+      </c>
+      <c r="B144" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D144" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E144" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F144" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="13">
+        <v>43233</v>
+      </c>
+      <c r="B145" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D145" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E145" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F145" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="13">
+        <v>43234</v>
+      </c>
+      <c r="B146" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Monday</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D146" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E146" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F146" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="13">
+        <v>43235</v>
+      </c>
+      <c r="B147" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D147" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E147" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F147" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="13">
+        <v>43236</v>
+      </c>
+      <c r="B148" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D148" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E148" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F148" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="13">
+        <v>43237</v>
+      </c>
+      <c r="B149" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D149" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E149" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F149" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="13">
+        <v>43238</v>
+      </c>
+      <c r="B150" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Friday</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D150" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E150" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F150" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="13">
+        <v>43239</v>
+      </c>
+      <c r="B151" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D151" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E151" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F151" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="13">
+        <v>43240</v>
+      </c>
+      <c r="B152" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E152" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F152" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="13">
+        <v>43241</v>
+      </c>
+      <c r="B153" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Monday</v>
+      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E153" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F153" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="13">
+        <v>43242</v>
+      </c>
+      <c r="B154" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C154" s="4"/>
+      <c r="D154" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E154" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F154" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="13">
+        <v>43243</v>
+      </c>
+      <c r="B155" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="C155" s="4"/>
+      <c r="D155" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E155" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F155" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="13">
+        <v>43244</v>
+      </c>
+      <c r="B156" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Thursday</v>
+      </c>
+      <c r="C156" s="4"/>
+      <c r="D156" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E156" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F156" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="13">
+        <v>43245</v>
+      </c>
+      <c r="B157" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Friday</v>
+      </c>
+      <c r="C157" s="4"/>
+      <c r="D157" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E157" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F157" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="13">
+        <v>43246</v>
+      </c>
+      <c r="B158" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C158" s="4"/>
+      <c r="D158" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E158" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F158" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="13">
+        <v>43247</v>
+      </c>
+      <c r="B159" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Sunday</v>
+      </c>
+      <c r="C159" s="4"/>
+      <c r="D159" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E159" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F159" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="13">
+        <v>43248</v>
+      </c>
+      <c r="B160" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>Monday</v>
+      </c>
+      <c r="C160" s="4"/>
+      <c r="D160" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E160" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F160" s="15">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" s="15" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -2095,7 +4080,7 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Foute datum" error="De datum moet liggen in het jaartal van de versie. Dus in de versie van 2018 kun je alleen mutaties uit 2018 vastleggen" sqref="A13:A72">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Foute datum" error="De datum moet liggen in het jaartal van de versie. Dus in de versie van 2018 kun je alleen mutaties uit 2018 vastleggen" sqref="A13:A160">
       <formula1>begin</formula1>
       <formula2>eind</formula2>
     </dataValidation>
@@ -2239,20 +4224,20 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="41.25" customHeight="1">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="18"/>
@@ -2292,20 +4277,20 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="27" customHeight="1">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
     </row>
     <row r="19" spans="2:13" ht="16">
       <c r="B19" s="20" t="s">
@@ -2313,46 +4298,46 @@
       </c>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="21"/>
@@ -2381,46 +4366,46 @@
       <c r="K24" s="22"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="21"/>
@@ -2449,32 +4434,32 @@
       <c r="K29" s="22"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" s="21"/>

</xml_diff>